<commit_message>
FHIR-35576 update DSTU2 to R4 Conversion Page
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/dstu2-r4-table.xlsx
+++ b/input/resources_spreadsheets/dstu2-r4-table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Argo-R4/source/source_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F91323EF-6767-484F-A089-83ED622B861E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DFC703-B469-3241-92C3-47C60F2F15A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
+    <workbookView xWindow="11620" yWindow="500" windowWidth="42400" windowHeight="27500" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>DSTU2 Profile</t>
   </si>
   <si>
-    <t>Equivalent R4 Profile</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -174,22 +171,133 @@
     <t>Type changed from CarePlan in DSTU2 to CareTeam in R4</t>
   </si>
   <si>
-    <t>New Profile in R4</t>
-  </si>
-  <si>
-    <t>New Profile in R4 based on the FHIR Vital Signs Profile</t>
-  </si>
-  <si>
-    <t>US Core MedicationStatement Profile not defined in R4</t>
-  </si>
-  <si>
-    <t>The FHIR core Vital Signs Profile</t>
-  </si>
-  <si>
-    <t>The FHIR Vital Signs Profile is published in the FHIR specificaition</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Version Added</t>
+  </si>
+  <si>
+    <t>Equivalent US Core Profile</t>
+  </si>
+  <si>
+    <t>3.1.1*</t>
+  </si>
+  <si>
+    <t>US Core Condition Encounter Diagnosis Profile</t>
+  </si>
+  <si>
+    <t>US Core Condition Problems and Health Concerns Profile</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>US Core DiagnosticReport Profile for Report and Note Exchange</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
+  </si>
+  <si>
+    <t>US Core Birth Sex Extension</t>
+  </si>
+  <si>
+    <t>US Core Direct email Extension</t>
+  </si>
+  <si>
+    <t>US Core Ethnicity Extension</t>
+  </si>
+  <si>
+    <t>US Core Race Extension</t>
+  </si>
+  <si>
+    <t>Argonaut Race Extension</t>
+  </si>
+  <si>
+    <t>Argonaut ethnicity Extension</t>
+  </si>
+  <si>
+    <t>Sex of patient assigned at birth</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>US Core Vital Signs Profile</t>
+  </si>
+  <si>
+    <t>US Core Blood Pressure Profile</t>
+  </si>
+  <si>
+    <t>US Core BMI Profile</t>
+  </si>
+  <si>
+    <t>US Core Head Circumference Profile</t>
+  </si>
+  <si>
+    <t>US Core Body Height Profile</t>
+  </si>
+  <si>
+    <t>US Core Body Weight Profile</t>
+  </si>
+  <si>
+    <t>US Core Body Temperature Profile</t>
+  </si>
+  <si>
+    <t>US Core Heart Rate Profile</t>
+  </si>
+  <si>
+    <t>US Core Respiratory Rate Profile</t>
+  </si>
+  <si>
+    <t>Previous to this version, referenced the FHIR Vital Signs Profile</t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>US Core Observation Sexual Orientation Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Social History Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Survey Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation SDOH Assessment Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Clinical Test Result Profile</t>
+  </si>
+  <si>
+    <t>US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t>US Core RelatedPerson Profile</t>
+  </si>
+  <si>
+    <t>US Core ServiceRequest Profile</t>
+  </si>
+  <si>
+    <t>US Core Extension Questionnaire URI</t>
+  </si>
+  <si>
+    <t>US Core Gender Identity Extension</t>
+  </si>
+  <si>
+    <t>**Extensions**</t>
+  </si>
+  <si>
+    <t>In version 5.0.0 split US Core Condition Profilee into US Core Condition Encounter Diagnosis Profile and US Core Condition Problems and Health Concerns Profile</t>
+  </si>
+  <si>
+    <t>US Core MedicationStatement Profile not defined in 3.1.1*</t>
+  </si>
+  <si>
+    <t>3.1.1* based on the FHIR Vital Signs Profile, 4.0.0+ based on the US Core Vital Signs Profile</t>
+  </si>
+  <si>
+    <t>\* 3.1.1  *or prior* version of US Core</t>
   </si>
 </sst>
 </file>
@@ -225,9 +333,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,291 +655,671 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E31E7FA-8383-CC4B-850A-1310B017638F}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FHIR-38702 add Coverage, update USCDI_v2_table_links and DSTU2_table_links, CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/dstu2-r4-table.xlsx
+++ b/input/resources_spreadsheets/dstu2-r4-table.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A11183-50F7-F84F-A8F0-56FF08CA892B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DADD82D-5CD5-D549-86AA-93D429B71FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11620" yWindow="500" windowWidth="42400" windowHeight="27500" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
+    <workbookView xWindow="-9820" yWindow="-28300" windowWidth="34120" windowHeight="28300" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
   <si>
     <t>DSTU2 Profile</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Argonaut Vital Signs Observation Profile</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
     <t>US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>US Core Respiratory Rate Profile</t>
   </si>
   <si>
-    <t>Previous to this version, referenced the FHIR Vital Signs Profile</t>
-  </si>
-  <si>
     <t>see above</t>
   </si>
   <si>
@@ -297,7 +291,37 @@
     <t>US Core Pediatric Head Occipital     -frontal Circumference Percentile Profile</t>
   </si>
   <si>
-    <t>: - - -:</t>
+    <t>US Core Coverage Profile</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Intent Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Occupation Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Status Profile</t>
+  </si>
+  <si>
+    <t>US Core MedicationDispense Profile</t>
+  </si>
+  <si>
+    <t>US Core Specimen Profile</t>
+  </si>
+  <si>
+    <t>US Core Sex Extension</t>
+  </si>
+  <si>
+    <t>Deprecated in 6.0.0</t>
+  </si>
+  <si>
+    <t>Previous to version 4.0.0, referenced the FHIR Vital Signs Profile</t>
+  </si>
+  <si>
+    <t>Previous to version 6.0.0, Use US Core Birth Sex Extension (deprecated)</t>
   </si>
 </sst>
 </file>
@@ -333,14 +357,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E31E7FA-8383-CC4B-850A-1310B017638F}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,660 +696,729 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
       <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
         <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
         <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>68</v>
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>86</v>
+      <c r="A30" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>86</v>
+      <c r="A32" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" t="s">
-        <v>30</v>
-      </c>
       <c r="C37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
         <v>86</v>
       </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="C48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
         <v>77</v>
       </c>
-      <c r="C47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="C60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
         <v>78</v>
       </c>
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C54" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
-        <v>85</v>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FHIR-38702 USCDI v3 changes to patient  deceased and tribe
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/dstu2-r4-table.xlsx
+++ b/input/resources_spreadsheets/dstu2-r4-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DADD82D-5CD5-D549-86AA-93D429B71FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6AF51C-A029-0049-81CE-556D90330595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9820" yWindow="-28300" windowWidth="34120" windowHeight="28300" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="98">
   <si>
     <t>DSTU2 Profile</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Previous to version 6.0.0, Use US Core Birth Sex Extension (deprecated)</t>
+  </si>
+  <si>
+    <t>US Core Tribal Affiliation Extension</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E31E7FA-8383-CC4B-850A-1310B017638F}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1420,18 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
+      <c r="A62" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix title for US Core Pediatric Head Occipital Frontal Circumference Observation Profile FHIR-38794
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/dstu2-r4-table.xlsx
+++ b/input/resources_spreadsheets/dstu2-r4-table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6AF51C-A029-0049-81CE-556D90330595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3E9175-11C1-8B41-ACB7-0E408D506A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="56640" windowHeight="21820" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t xml:space="preserve">     -</t>
   </si>
   <si>
-    <t>US Core Pediatric Head Occipital     -frontal Circumference Percentile Profile</t>
-  </si>
-  <si>
     <t>US Core Coverage Profile</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>US Core Tribal Affiliation Extension</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
   </si>
 </sst>
 </file>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E31E7FA-8383-CC4B-850A-1310B017638F}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,7 +929,7 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -957,7 +957,7 @@
         <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,7 +1041,7 @@
         <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1063,7 +1063,7 @@
         <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
@@ -1270,10 +1270,10 @@
         <v>84</v>
       </c>
       <c r="B48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" t="s">
         <v>86</v>
-      </c>
-      <c r="C48" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1281,10 +1281,10 @@
         <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1292,10 +1292,10 @@
         <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1303,10 +1303,10 @@
         <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1314,10 +1314,10 @@
         <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,10 +1325,10 @@
         <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1347,7 +1347,7 @@
         <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1355,13 +1355,13 @@
         <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1424,10 +1424,10 @@
         <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>